<commit_message>
[IMP] Adjust SLA Receipt Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_sla_receipt.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_sla_receipt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SLA Receipt Report" sheetId="1" state="visible" r:id="rId2"/>
@@ -1480,7 +1480,7 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00_);\(#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
   <fonts count="7">
@@ -1727,23 +1727,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:11"/>
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="22.3979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="23.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="26.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.719387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="21.2397959183673"/>
-    <col collapsed="false" hidden="false" max="1010" min="9" style="4" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="1011" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="22.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="26.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="27.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="21.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1010" min="9" style="4" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1011" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11931,7 +11931,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -11946,15 +11946,15 @@
   </sheetPr>
   <dimension ref="A1:B459"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15019,7 +15019,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>